<commit_message>
more analysis on fsr4
</commit_message>
<xml_diff>
--- a/data/FSR_S4/stability/FSR_S4 Stability Data.xlsx
+++ b/data/FSR_S4/stability/FSR_S4 Stability Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrickruiz/Desktop/FSR/data/FSR_S4/stability/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F0A26D-383C-5B42-998D-86C2883E95DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{201BA6D9-692A-5D48-AA5C-6B9913F18A18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="22500" xr2:uid="{05FAEE67-03BB-4EED-BB39-2994B23103BF}"/>
   </bookViews>
@@ -432,7 +432,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="167" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H22"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>